<commit_message>
add flujos transferencia propia
</commit_message>
<xml_diff>
--- a/Automatizacion BEL Web/Datos.xlsx
+++ b/Automatizacion BEL Web/Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\67847\Downloads\bautomata-master\Automatizacion BEL Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\63839\Documents\BITesting-DesignSprint2.0\Automatizacion BEL Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7369B0-D869-40A3-A961-C1279EE1BA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0065E35-D106-4996-81E1-A95948056F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0029890E-033D-4DFF-ADD2-A02E36070D60}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0029890E-033D-4DFF-ADD2-A02E36070D60}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -226,10 +226,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -567,21 +567,21 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -589,23 +589,23 @@
         <v>163001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>112233</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -632,18 +632,18 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="4"/>
-    <col min="4" max="4" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="4"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -657,13 +657,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="D2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="D3" t="s">
         <v>23</v>
@@ -684,15 +684,15 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38.77734375" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -706,11 +706,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -741,15 +741,15 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="4"/>
-    <col min="4" max="4" width="38.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="4"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -763,22 +763,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
     </row>
   </sheetData>
@@ -795,52 +795,52 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>

</xml_diff>